<commit_message>
update final template 1900
</commit_message>
<xml_diff>
--- a/blocks/1908/TestCase-Module -1908.xlsx
+++ b/blocks/1908/TestCase-Module -1908.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\template1900\blocks\1908\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20388" windowHeight="8352" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20388" windowHeight="8352" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -454,9 +454,6 @@
     <t>Hình 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Block 1902 </t>
-  </si>
-  <si>
     <t>- Danh mục trong trường hợp không có dữ liệu</t>
   </si>
   <si>
@@ -644,6 +641,9 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block 1908 </t>
   </si>
 </sst>
 </file>
@@ -1279,30 +1279,69 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="5" xfId="5" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="5" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1330,41 +1369,14 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="5" xfId="5" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1375,6 +1387,171 @@
     <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="5" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1389,183 +1566,6 @@
     </xf>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="16" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="5" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -3473,35 +3473,35 @@
       <c r="M17" s="45"/>
       <c r="N17" s="45"/>
       <c r="O17" s="45"/>
-      <c r="P17" s="71"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="71"/>
-      <c r="S17" s="71"/>
-      <c r="T17" s="71"/>
-      <c r="U17" s="71"/>
-      <c r="V17" s="72"/>
-      <c r="W17" s="72"/>
-      <c r="X17" s="72"/>
-      <c r="Y17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="72"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="72"/>
+      <c r="U17" s="72"/>
+      <c r="V17" s="73"/>
+      <c r="W17" s="73"/>
+      <c r="X17" s="73"/>
+      <c r="Y17" s="73"/>
       <c r="Z17" s="45"/>
       <c r="AA17" s="45"/>
       <c r="AB17" s="45"/>
       <c r="AC17" s="45"/>
       <c r="AD17" s="45"/>
       <c r="AE17" s="45"/>
-      <c r="AF17" s="71"/>
-      <c r="AG17" s="72"/>
-      <c r="AH17" s="72"/>
-      <c r="AI17" s="72"/>
-      <c r="AJ17" s="72"/>
-      <c r="AK17" s="72"/>
-      <c r="AL17" s="72"/>
-      <c r="AM17" s="72"/>
-      <c r="AN17" s="72"/>
-      <c r="AO17" s="72"/>
-      <c r="AP17" s="72"/>
-      <c r="AQ17" s="72"/>
-      <c r="AR17" s="72"/>
+      <c r="AF17" s="72"/>
+      <c r="AG17" s="73"/>
+      <c r="AH17" s="73"/>
+      <c r="AI17" s="73"/>
+      <c r="AJ17" s="73"/>
+      <c r="AK17" s="73"/>
+      <c r="AL17" s="73"/>
+      <c r="AM17" s="73"/>
+      <c r="AN17" s="73"/>
+      <c r="AO17" s="73"/>
+      <c r="AP17" s="73"/>
+      <c r="AQ17" s="73"/>
+      <c r="AR17" s="73"/>
       <c r="AS17" s="45"/>
       <c r="AT17" s="45"/>
       <c r="AU17" s="45"/>
@@ -3709,16 +3709,16 @@
       <c r="M21" s="45"/>
       <c r="N21" s="45"/>
       <c r="O21" s="45"/>
-      <c r="P21" s="71"/>
-      <c r="Q21" s="71"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="71"/>
-      <c r="T21" s="71"/>
-      <c r="U21" s="71"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="71"/>
-      <c r="Y21" s="71"/>
+      <c r="P21" s="72"/>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="72"/>
+      <c r="T21" s="72"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="72"/>
+      <c r="W21" s="72"/>
+      <c r="X21" s="72"/>
+      <c r="Y21" s="72"/>
       <c r="Z21" s="45"/>
       <c r="AA21" s="45"/>
       <c r="AB21" s="45"/>
@@ -4759,9 +4759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.296875" defaultRowHeight="13.2"/>
   <cols>
@@ -4775,7 +4773,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="19" customFormat="1" ht="23.4">
       <c r="A1" s="24" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24" t="s">
@@ -4803,11 +4801,11 @@
       <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="166" t="s">
-        <v>43</v>
+      <c r="B3" s="71" t="s">
+        <v>42</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="33">
         <v>43613</v>
@@ -4967,7 +4965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="BA6" sqref="BA6:BH7"/>
     </sheetView>
   </sheetViews>
@@ -4981,286 +4979,286 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="160" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="124" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
+      <c r="Y1" s="118"/>
+      <c r="Z1" s="118"/>
+      <c r="AA1" s="118"/>
+      <c r="AB1" s="118"/>
+      <c r="AC1" s="118"/>
+      <c r="AD1" s="118"/>
+      <c r="AE1" s="118"/>
+      <c r="AF1" s="118"/>
+      <c r="AG1" s="118"/>
+      <c r="AH1" s="118"/>
+      <c r="AI1" s="119"/>
+      <c r="AJ1" s="125" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK1" s="126"/>
+      <c r="AL1" s="126"/>
+      <c r="AM1" s="126"/>
+      <c r="AN1" s="127" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO1" s="125"/>
+      <c r="AP1" s="126"/>
+      <c r="AQ1" s="126"/>
+      <c r="AR1" s="126"/>
+      <c r="AS1" s="127" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT1" s="126"/>
+      <c r="AU1" s="126"/>
+      <c r="AV1" s="126"/>
+      <c r="AW1" s="110" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX1" s="111"/>
+      <c r="AY1" s="111"/>
+      <c r="AZ1" s="112"/>
+      <c r="BA1" s="113" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB1" s="113"/>
+      <c r="BC1" s="113"/>
+      <c r="BD1" s="113"/>
+      <c r="BE1" s="113"/>
+      <c r="BF1" s="113"/>
+      <c r="BG1" s="113"/>
+      <c r="BH1" s="113"/>
+      <c r="BI1" s="15"/>
+    </row>
+    <row r="2" spans="1:61">
+      <c r="A2" s="114"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="118"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="118"/>
+      <c r="AA2" s="118"/>
+      <c r="AB2" s="118"/>
+      <c r="AC2" s="118"/>
+      <c r="AD2" s="118"/>
+      <c r="AE2" s="118"/>
+      <c r="AF2" s="118"/>
+      <c r="AG2" s="118"/>
+      <c r="AH2" s="118"/>
+      <c r="AI2" s="119"/>
+      <c r="AJ2" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="154"/>
-      <c r="O1" s="154"/>
-      <c r="P1" s="154"/>
-      <c r="Q1" s="154"/>
-      <c r="R1" s="154"/>
-      <c r="S1" s="154"/>
-      <c r="T1" s="154"/>
-      <c r="U1" s="154"/>
-      <c r="V1" s="154"/>
-      <c r="W1" s="154"/>
-      <c r="X1" s="154"/>
-      <c r="Y1" s="154"/>
-      <c r="Z1" s="154"/>
-      <c r="AA1" s="154"/>
-      <c r="AB1" s="154"/>
-      <c r="AC1" s="154"/>
-      <c r="AD1" s="154"/>
-      <c r="AE1" s="154"/>
-      <c r="AF1" s="154"/>
-      <c r="AG1" s="154"/>
-      <c r="AH1" s="154"/>
-      <c r="AI1" s="155"/>
-      <c r="AJ1" s="161" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK1" s="162"/>
-      <c r="AL1" s="162"/>
-      <c r="AM1" s="162"/>
-      <c r="AN1" s="163" t="s">
-        <v>9</v>
-      </c>
-      <c r="AO1" s="161"/>
-      <c r="AP1" s="162"/>
-      <c r="AQ1" s="162"/>
-      <c r="AR1" s="162"/>
-      <c r="AS1" s="163" t="s">
-        <v>10</v>
-      </c>
-      <c r="AT1" s="162"/>
-      <c r="AU1" s="162"/>
-      <c r="AV1" s="162"/>
-      <c r="AW1" s="131" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX1" s="132"/>
-      <c r="AY1" s="132"/>
-      <c r="AZ1" s="133"/>
-      <c r="BA1" s="152" t="s">
-        <v>11</v>
-      </c>
-      <c r="BB1" s="152"/>
-      <c r="BC1" s="152"/>
-      <c r="BD1" s="152"/>
-      <c r="BE1" s="152"/>
-      <c r="BF1" s="152"/>
-      <c r="BG1" s="152"/>
-      <c r="BH1" s="152"/>
-      <c r="BI1" s="15"/>
-    </row>
-    <row r="2" spans="1:61">
-      <c r="A2" s="143"/>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="154"/>
-      <c r="S2" s="154"/>
-      <c r="T2" s="154"/>
-      <c r="U2" s="154"/>
-      <c r="V2" s="154"/>
-      <c r="W2" s="154"/>
-      <c r="X2" s="154"/>
-      <c r="Y2" s="154"/>
-      <c r="Z2" s="154"/>
-      <c r="AA2" s="154"/>
-      <c r="AB2" s="154"/>
-      <c r="AC2" s="154"/>
-      <c r="AD2" s="154"/>
-      <c r="AE2" s="154"/>
-      <c r="AF2" s="154"/>
-      <c r="AG2" s="154"/>
-      <c r="AH2" s="154"/>
-      <c r="AI2" s="155"/>
-      <c r="AJ2" s="156" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK2" s="157"/>
-      <c r="AL2" s="157"/>
-      <c r="AM2" s="157"/>
-      <c r="AN2" s="158" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO2" s="156"/>
-      <c r="AP2" s="157"/>
-      <c r="AQ2" s="157"/>
-      <c r="AR2" s="157"/>
-      <c r="AS2" s="158">
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121"/>
+      <c r="AN2" s="122" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO2" s="120"/>
+      <c r="AP2" s="121"/>
+      <c r="AQ2" s="121"/>
+      <c r="AR2" s="121"/>
+      <c r="AS2" s="122">
         <f>COUNTIF($AR:$AR,"NG")</f>
         <v>0</v>
       </c>
-      <c r="AT2" s="157"/>
-      <c r="AU2" s="157"/>
-      <c r="AV2" s="157"/>
-      <c r="AW2" s="131" t="s">
+      <c r="AT2" s="121"/>
+      <c r="AU2" s="121"/>
+      <c r="AV2" s="121"/>
+      <c r="AW2" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="AX2" s="132"/>
-      <c r="AY2" s="132"/>
-      <c r="AZ2" s="133"/>
-      <c r="BA2" s="159" t="s">
+      <c r="AX2" s="111"/>
+      <c r="AY2" s="111"/>
+      <c r="AZ2" s="112"/>
+      <c r="BA2" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="BB2" s="152"/>
-      <c r="BC2" s="152"/>
-      <c r="BD2" s="152"/>
-      <c r="BE2" s="152"/>
-      <c r="BF2" s="152"/>
-      <c r="BG2" s="152"/>
-      <c r="BH2" s="152"/>
+      <c r="BB2" s="113"/>
+      <c r="BC2" s="113"/>
+      <c r="BD2" s="113"/>
+      <c r="BE2" s="113"/>
+      <c r="BF2" s="113"/>
+      <c r="BG2" s="113"/>
+      <c r="BH2" s="113"/>
       <c r="BI2" s="15"/>
     </row>
     <row r="3" spans="1:61">
-      <c r="A3" s="108"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
-      <c r="N3" s="115"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
-      <c r="S3" s="115"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="115"/>
-      <c r="V3" s="115"/>
-      <c r="W3" s="115"/>
-      <c r="X3" s="115"/>
-      <c r="Y3" s="115"/>
-      <c r="Z3" s="115"/>
-      <c r="AA3" s="115"/>
-      <c r="AB3" s="115"/>
-      <c r="AC3" s="115"/>
-      <c r="AD3" s="115"/>
-      <c r="AE3" s="115"/>
-      <c r="AF3" s="115"/>
-      <c r="AG3" s="115"/>
-      <c r="AH3" s="115"/>
-      <c r="AI3" s="116"/>
-      <c r="AJ3" s="131" t="s">
+      <c r="A3" s="148"/>
+      <c r="B3" s="149"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="155"/>
+      <c r="J3" s="155"/>
+      <c r="K3" s="155"/>
+      <c r="L3" s="155"/>
+      <c r="M3" s="155"/>
+      <c r="N3" s="155"/>
+      <c r="O3" s="155"/>
+      <c r="P3" s="155"/>
+      <c r="Q3" s="155"/>
+      <c r="R3" s="155"/>
+      <c r="S3" s="155"/>
+      <c r="T3" s="155"/>
+      <c r="U3" s="155"/>
+      <c r="V3" s="155"/>
+      <c r="W3" s="155"/>
+      <c r="X3" s="155"/>
+      <c r="Y3" s="155"/>
+      <c r="Z3" s="155"/>
+      <c r="AA3" s="155"/>
+      <c r="AB3" s="155"/>
+      <c r="AC3" s="155"/>
+      <c r="AD3" s="155"/>
+      <c r="AE3" s="155"/>
+      <c r="AF3" s="155"/>
+      <c r="AG3" s="155"/>
+      <c r="AH3" s="155"/>
+      <c r="AI3" s="156"/>
+      <c r="AJ3" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="AK3" s="132"/>
-      <c r="AL3" s="132"/>
-      <c r="AM3" s="133"/>
-      <c r="AN3" s="140"/>
-      <c r="AO3" s="141"/>
-      <c r="AP3" s="141"/>
-      <c r="AQ3" s="141"/>
-      <c r="AR3" s="141"/>
-      <c r="AS3" s="141"/>
-      <c r="AT3" s="141"/>
-      <c r="AU3" s="141"/>
-      <c r="AV3" s="142"/>
-      <c r="AW3" s="131"/>
-      <c r="AX3" s="132"/>
-      <c r="AY3" s="132"/>
-      <c r="AZ3" s="133"/>
-      <c r="BA3" s="140"/>
-      <c r="BB3" s="141"/>
-      <c r="BC3" s="141"/>
-      <c r="BD3" s="141"/>
-      <c r="BE3" s="141"/>
-      <c r="BF3" s="141"/>
-      <c r="BG3" s="141"/>
-      <c r="BH3" s="142"/>
+      <c r="AK3" s="111"/>
+      <c r="AL3" s="111"/>
+      <c r="AM3" s="112"/>
+      <c r="AN3" s="128"/>
+      <c r="AO3" s="129"/>
+      <c r="AP3" s="129"/>
+      <c r="AQ3" s="129"/>
+      <c r="AR3" s="129"/>
+      <c r="AS3" s="129"/>
+      <c r="AT3" s="129"/>
+      <c r="AU3" s="129"/>
+      <c r="AV3" s="130"/>
+      <c r="AW3" s="110"/>
+      <c r="AX3" s="111"/>
+      <c r="AY3" s="111"/>
+      <c r="AZ3" s="112"/>
+      <c r="BA3" s="128"/>
+      <c r="BB3" s="129"/>
+      <c r="BC3" s="129"/>
+      <c r="BD3" s="129"/>
+      <c r="BE3" s="129"/>
+      <c r="BF3" s="129"/>
+      <c r="BG3" s="129"/>
+      <c r="BH3" s="130"/>
       <c r="BI3" s="15"/>
     </row>
     <row r="4" spans="1:61">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="118"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118"/>
-      <c r="Q4" s="118"/>
-      <c r="R4" s="118"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="118"/>
-      <c r="X4" s="118"/>
-      <c r="Y4" s="118"/>
-      <c r="Z4" s="118"/>
-      <c r="AA4" s="118"/>
-      <c r="AB4" s="118"/>
-      <c r="AC4" s="118"/>
-      <c r="AD4" s="118"/>
-      <c r="AE4" s="118"/>
-      <c r="AF4" s="118"/>
-      <c r="AG4" s="118"/>
-      <c r="AH4" s="118"/>
-      <c r="AI4" s="119"/>
-      <c r="AJ4" s="143" t="s">
+      <c r="A4" s="151"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="157"/>
+      <c r="I4" s="158"/>
+      <c r="J4" s="158"/>
+      <c r="K4" s="158"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="158"/>
+      <c r="N4" s="158"/>
+      <c r="O4" s="158"/>
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
+      <c r="S4" s="158"/>
+      <c r="T4" s="158"/>
+      <c r="U4" s="158"/>
+      <c r="V4" s="158"/>
+      <c r="W4" s="158"/>
+      <c r="X4" s="158"/>
+      <c r="Y4" s="158"/>
+      <c r="Z4" s="158"/>
+      <c r="AA4" s="158"/>
+      <c r="AB4" s="158"/>
+      <c r="AC4" s="158"/>
+      <c r="AD4" s="158"/>
+      <c r="AE4" s="158"/>
+      <c r="AF4" s="158"/>
+      <c r="AG4" s="158"/>
+      <c r="AH4" s="158"/>
+      <c r="AI4" s="159"/>
+      <c r="AJ4" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="144"/>
-      <c r="AL4" s="144"/>
-      <c r="AM4" s="145"/>
-      <c r="AN4" s="146"/>
-      <c r="AO4" s="147"/>
-      <c r="AP4" s="147"/>
-      <c r="AQ4" s="147"/>
-      <c r="AR4" s="147"/>
-      <c r="AS4" s="147"/>
-      <c r="AT4" s="147"/>
-      <c r="AU4" s="147"/>
-      <c r="AV4" s="148"/>
-      <c r="AW4" s="143" t="s">
+      <c r="AK4" s="115"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="116"/>
+      <c r="AN4" s="131"/>
+      <c r="AO4" s="132"/>
+      <c r="AP4" s="132"/>
+      <c r="AQ4" s="132"/>
+      <c r="AR4" s="132"/>
+      <c r="AS4" s="132"/>
+      <c r="AT4" s="132"/>
+      <c r="AU4" s="132"/>
+      <c r="AV4" s="133"/>
+      <c r="AW4" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="AX4" s="144"/>
-      <c r="AY4" s="144"/>
-      <c r="AZ4" s="145"/>
-      <c r="BA4" s="146"/>
-      <c r="BB4" s="147"/>
-      <c r="BC4" s="147"/>
-      <c r="BD4" s="147"/>
-      <c r="BE4" s="147"/>
-      <c r="BF4" s="147"/>
-      <c r="BG4" s="147"/>
-      <c r="BH4" s="148"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115"/>
+      <c r="AZ4" s="116"/>
+      <c r="BA4" s="131"/>
+      <c r="BB4" s="132"/>
+      <c r="BC4" s="132"/>
+      <c r="BD4" s="132"/>
+      <c r="BE4" s="132"/>
+      <c r="BF4" s="132"/>
+      <c r="BG4" s="132"/>
+      <c r="BH4" s="133"/>
     </row>
     <row r="5" spans="1:61" s="10" customFormat="1">
       <c r="A5" s="14"/>
@@ -5326,1218 +5324,1234 @@
       <c r="BI5" s="14"/>
     </row>
     <row r="6" spans="1:61" ht="14.4">
-      <c r="A6" s="120" t="s">
+      <c r="A6" s="160" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="120"/>
-      <c r="C6" s="134" t="s">
+      <c r="B6" s="160"/>
+      <c r="C6" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="122" t="s">
+      <c r="D6" s="137"/>
+      <c r="E6" s="137"/>
+      <c r="F6" s="137"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="137"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="137"/>
+      <c r="M6" s="137"/>
+      <c r="N6" s="137"/>
+      <c r="O6" s="137"/>
+      <c r="P6" s="137"/>
+      <c r="Q6" s="137"/>
+      <c r="R6" s="137"/>
+      <c r="S6" s="137"/>
+      <c r="T6" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="U6" s="123"/>
-      <c r="V6" s="123"/>
-      <c r="W6" s="123"/>
-      <c r="X6" s="123"/>
-      <c r="Y6" s="123"/>
-      <c r="Z6" s="123"/>
-      <c r="AA6" s="123"/>
-      <c r="AB6" s="124"/>
-      <c r="AC6" s="122" t="s">
+      <c r="U6" s="142"/>
+      <c r="V6" s="142"/>
+      <c r="W6" s="142"/>
+      <c r="X6" s="142"/>
+      <c r="Y6" s="142"/>
+      <c r="Z6" s="142"/>
+      <c r="AA6" s="142"/>
+      <c r="AB6" s="143"/>
+      <c r="AC6" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="AD6" s="123"/>
-      <c r="AE6" s="123"/>
-      <c r="AF6" s="123"/>
-      <c r="AG6" s="123"/>
-      <c r="AH6" s="123"/>
-      <c r="AI6" s="123"/>
-      <c r="AJ6" s="123"/>
-      <c r="AK6" s="123"/>
-      <c r="AL6" s="123"/>
-      <c r="AM6" s="124"/>
-      <c r="AN6" s="122" t="s">
+      <c r="AD6" s="142"/>
+      <c r="AE6" s="142"/>
+      <c r="AF6" s="142"/>
+      <c r="AG6" s="142"/>
+      <c r="AH6" s="142"/>
+      <c r="AI6" s="142"/>
+      <c r="AJ6" s="142"/>
+      <c r="AK6" s="142"/>
+      <c r="AL6" s="142"/>
+      <c r="AM6" s="143"/>
+      <c r="AN6" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AO6" s="123"/>
-      <c r="AP6" s="123"/>
-      <c r="AQ6" s="124"/>
-      <c r="AR6" s="122" t="s">
+      <c r="AO6" s="142"/>
+      <c r="AP6" s="142"/>
+      <c r="AQ6" s="143"/>
+      <c r="AR6" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="AS6" s="123"/>
-      <c r="AT6" s="124"/>
-      <c r="AU6" s="122" t="s">
+      <c r="AS6" s="142"/>
+      <c r="AT6" s="143"/>
+      <c r="AU6" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="AV6" s="123"/>
-      <c r="AW6" s="124"/>
-      <c r="AX6" s="122" t="s">
+      <c r="AV6" s="142"/>
+      <c r="AW6" s="143"/>
+      <c r="AX6" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="AY6" s="123"/>
-      <c r="AZ6" s="124"/>
-      <c r="BA6" s="139" t="s">
+      <c r="AY6" s="142"/>
+      <c r="AZ6" s="143"/>
+      <c r="BA6" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="BB6" s="139"/>
-      <c r="BC6" s="139"/>
-      <c r="BD6" s="139"/>
-      <c r="BE6" s="139"/>
-      <c r="BF6" s="139"/>
-      <c r="BG6" s="139"/>
-      <c r="BH6" s="139"/>
+      <c r="BB6" s="147"/>
+      <c r="BC6" s="147"/>
+      <c r="BD6" s="147"/>
+      <c r="BE6" s="147"/>
+      <c r="BF6" s="147"/>
+      <c r="BG6" s="147"/>
+      <c r="BH6" s="147"/>
       <c r="BI6" s="16"/>
     </row>
     <row r="7" spans="1:61" s="11" customFormat="1" ht="14.4">
-      <c r="A7" s="121"/>
-      <c r="B7" s="121"/>
-      <c r="C7" s="136" t="s">
+      <c r="A7" s="161"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="137" t="s">
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="137"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="137"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="138" t="s">
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="139"/>
+      <c r="M7" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="135"/>
-      <c r="R7" s="135"/>
-      <c r="S7" s="135"/>
-      <c r="T7" s="125"/>
-      <c r="U7" s="126"/>
-      <c r="V7" s="126"/>
-      <c r="W7" s="126"/>
-      <c r="X7" s="126"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="126"/>
-      <c r="AA7" s="126"/>
-      <c r="AB7" s="127"/>
-      <c r="AC7" s="125"/>
-      <c r="AD7" s="126"/>
-      <c r="AE7" s="126"/>
-      <c r="AF7" s="126"/>
-      <c r="AG7" s="126"/>
-      <c r="AH7" s="126"/>
-      <c r="AI7" s="126"/>
-      <c r="AJ7" s="126"/>
-      <c r="AK7" s="126"/>
-      <c r="AL7" s="126"/>
-      <c r="AM7" s="127"/>
-      <c r="AN7" s="125"/>
-      <c r="AO7" s="126"/>
-      <c r="AP7" s="126"/>
-      <c r="AQ7" s="127"/>
-      <c r="AR7" s="125"/>
-      <c r="AS7" s="126"/>
-      <c r="AT7" s="127"/>
-      <c r="AU7" s="125"/>
-      <c r="AV7" s="126"/>
-      <c r="AW7" s="127"/>
-      <c r="AX7" s="125"/>
-      <c r="AY7" s="126"/>
-      <c r="AZ7" s="127"/>
-      <c r="BA7" s="139"/>
-      <c r="BB7" s="139"/>
-      <c r="BC7" s="139"/>
-      <c r="BD7" s="139"/>
-      <c r="BE7" s="139"/>
-      <c r="BF7" s="139"/>
-      <c r="BG7" s="139"/>
-      <c r="BH7" s="139"/>
+      <c r="N7" s="137"/>
+      <c r="O7" s="137"/>
+      <c r="P7" s="137"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="137"/>
+      <c r="S7" s="137"/>
+      <c r="T7" s="144"/>
+      <c r="U7" s="145"/>
+      <c r="V7" s="145"/>
+      <c r="W7" s="145"/>
+      <c r="X7" s="145"/>
+      <c r="Y7" s="145"/>
+      <c r="Z7" s="145"/>
+      <c r="AA7" s="145"/>
+      <c r="AB7" s="146"/>
+      <c r="AC7" s="144"/>
+      <c r="AD7" s="145"/>
+      <c r="AE7" s="145"/>
+      <c r="AF7" s="145"/>
+      <c r="AG7" s="145"/>
+      <c r="AH7" s="145"/>
+      <c r="AI7" s="145"/>
+      <c r="AJ7" s="145"/>
+      <c r="AK7" s="145"/>
+      <c r="AL7" s="145"/>
+      <c r="AM7" s="146"/>
+      <c r="AN7" s="144"/>
+      <c r="AO7" s="145"/>
+      <c r="AP7" s="145"/>
+      <c r="AQ7" s="146"/>
+      <c r="AR7" s="144"/>
+      <c r="AS7" s="145"/>
+      <c r="AT7" s="146"/>
+      <c r="AU7" s="144"/>
+      <c r="AV7" s="145"/>
+      <c r="AW7" s="146"/>
+      <c r="AX7" s="144"/>
+      <c r="AY7" s="145"/>
+      <c r="AZ7" s="146"/>
+      <c r="BA7" s="147"/>
+      <c r="BB7" s="147"/>
+      <c r="BC7" s="147"/>
+      <c r="BD7" s="147"/>
+      <c r="BE7" s="147"/>
+      <c r="BF7" s="147"/>
+      <c r="BG7" s="147"/>
+      <c r="BH7" s="147"/>
       <c r="BI7" s="17"/>
     </row>
     <row r="8" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A8" s="88">
+      <c r="A8" s="74">
         <v>1</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="92" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="92" t="s">
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="98" t="s">
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="85"/>
+      <c r="Q8" s="85"/>
+      <c r="R8" s="85"/>
+      <c r="S8" s="86"/>
+      <c r="T8" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="73" t="s">
+      <c r="U8" s="85"/>
+      <c r="V8" s="85"/>
+      <c r="W8" s="85"/>
+      <c r="X8" s="85"/>
+      <c r="Y8" s="85"/>
+      <c r="Z8" s="85"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="U8" s="74"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="74"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="74"/>
-      <c r="AA8" s="74"/>
-      <c r="AB8" s="74"/>
-      <c r="AC8" s="77" t="s">
+      <c r="AD8" s="85"/>
+      <c r="AE8" s="85"/>
+      <c r="AF8" s="85"/>
+      <c r="AG8" s="85"/>
+      <c r="AH8" s="85"/>
+      <c r="AI8" s="85"/>
+      <c r="AJ8" s="85"/>
+      <c r="AK8" s="85"/>
+      <c r="AL8" s="85"/>
+      <c r="AM8" s="86"/>
+      <c r="AN8" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO8" s="96"/>
+      <c r="AP8" s="96"/>
+      <c r="AQ8" s="97"/>
+      <c r="AR8" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS8" s="96"/>
+      <c r="AT8" s="97"/>
+      <c r="AU8" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="AD8" s="74"/>
-      <c r="AE8" s="74"/>
-      <c r="AF8" s="74"/>
-      <c r="AG8" s="74"/>
-      <c r="AH8" s="74"/>
-      <c r="AI8" s="74"/>
-      <c r="AJ8" s="74"/>
-      <c r="AK8" s="74"/>
-      <c r="AL8" s="74"/>
-      <c r="AM8" s="78"/>
-      <c r="AN8" s="82" t="s">
+      <c r="AV8" s="96"/>
+      <c r="AW8" s="97"/>
+      <c r="AX8" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY8" s="96"/>
+      <c r="AZ8" s="97"/>
+      <c r="BA8" s="104" t="s">
+        <v>30</v>
+      </c>
+      <c r="BB8" s="105"/>
+      <c r="BC8" s="105"/>
+      <c r="BD8" s="105"/>
+      <c r="BE8" s="105"/>
+      <c r="BF8" s="105"/>
+      <c r="BG8" s="105"/>
+      <c r="BH8" s="106"/>
+      <c r="BI8" s="18"/>
+    </row>
+    <row r="9" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A9" s="76"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="88"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
+      <c r="X9" s="87"/>
+      <c r="Y9" s="87"/>
+      <c r="Z9" s="87"/>
+      <c r="AA9" s="87"/>
+      <c r="AB9" s="87"/>
+      <c r="AC9" s="92"/>
+      <c r="AD9" s="93"/>
+      <c r="AE9" s="93"/>
+      <c r="AF9" s="93"/>
+      <c r="AG9" s="93"/>
+      <c r="AH9" s="93"/>
+      <c r="AI9" s="93"/>
+      <c r="AJ9" s="93"/>
+      <c r="AK9" s="93"/>
+      <c r="AL9" s="93"/>
+      <c r="AM9" s="94"/>
+      <c r="AN9" s="98"/>
+      <c r="AO9" s="99"/>
+      <c r="AP9" s="99"/>
+      <c r="AQ9" s="100"/>
+      <c r="AR9" s="98"/>
+      <c r="AS9" s="99"/>
+      <c r="AT9" s="100"/>
+      <c r="AU9" s="98"/>
+      <c r="AV9" s="99"/>
+      <c r="AW9" s="100"/>
+      <c r="AX9" s="98"/>
+      <c r="AY9" s="99"/>
+      <c r="AZ9" s="100"/>
+      <c r="BA9" s="162"/>
+      <c r="BB9" s="163"/>
+      <c r="BC9" s="163"/>
+      <c r="BD9" s="163"/>
+      <c r="BE9" s="163"/>
+      <c r="BF9" s="163"/>
+      <c r="BG9" s="163"/>
+      <c r="BH9" s="164"/>
+      <c r="BI9" s="18"/>
+    </row>
+    <row r="10" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A10" s="74">
+        <v>2</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="84" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="85"/>
+      <c r="O10" s="85"/>
+      <c r="P10" s="85"/>
+      <c r="Q10" s="85"/>
+      <c r="R10" s="85"/>
+      <c r="S10" s="86"/>
+      <c r="T10" s="89" t="s">
+        <v>45</v>
+      </c>
+      <c r="U10" s="85"/>
+      <c r="V10" s="85"/>
+      <c r="W10" s="85"/>
+      <c r="X10" s="85"/>
+      <c r="Y10" s="85"/>
+      <c r="Z10" s="85"/>
+      <c r="AA10" s="85"/>
+      <c r="AB10" s="85"/>
+      <c r="AC10" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD10" s="85"/>
+      <c r="AE10" s="85"/>
+      <c r="AF10" s="85"/>
+      <c r="AG10" s="85"/>
+      <c r="AH10" s="85"/>
+      <c r="AI10" s="85"/>
+      <c r="AJ10" s="85"/>
+      <c r="AK10" s="85"/>
+      <c r="AL10" s="85"/>
+      <c r="AM10" s="86"/>
+      <c r="AN10" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="AO8" s="83"/>
-      <c r="AP8" s="83"/>
-      <c r="AQ8" s="84"/>
-      <c r="AR8" s="82" t="s">
+      <c r="AO10" s="96"/>
+      <c r="AP10" s="96"/>
+      <c r="AQ10" s="97"/>
+      <c r="AR10" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="AS8" s="83"/>
-      <c r="AT8" s="84"/>
-      <c r="AU8" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV8" s="83"/>
-      <c r="AW8" s="84"/>
-      <c r="AX8" s="82" t="s">
+      <c r="AS10" s="96"/>
+      <c r="AT10" s="97"/>
+      <c r="AU10" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV10" s="96"/>
+      <c r="AW10" s="97"/>
+      <c r="AX10" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="AY8" s="83"/>
-      <c r="AZ8" s="84"/>
-      <c r="BA8" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="BB8" s="101"/>
-      <c r="BC8" s="101"/>
-      <c r="BD8" s="101"/>
-      <c r="BE8" s="101"/>
-      <c r="BF8" s="101"/>
-      <c r="BG8" s="101"/>
-      <c r="BH8" s="102"/>
-      <c r="BI8" s="18"/>
-    </row>
-    <row r="9" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A9" s="90"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="128"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="128"/>
-      <c r="I9" s="129"/>
-      <c r="J9" s="129"/>
-      <c r="K9" s="129"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="99"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="76"/>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="76"/>
-      <c r="AC9" s="79"/>
-      <c r="AD9" s="80"/>
-      <c r="AE9" s="80"/>
-      <c r="AF9" s="80"/>
-      <c r="AG9" s="80"/>
-      <c r="AH9" s="80"/>
-      <c r="AI9" s="80"/>
-      <c r="AJ9" s="80"/>
-      <c r="AK9" s="80"/>
-      <c r="AL9" s="80"/>
-      <c r="AM9" s="81"/>
-      <c r="AN9" s="85"/>
-      <c r="AO9" s="86"/>
-      <c r="AP9" s="86"/>
-      <c r="AQ9" s="87"/>
-      <c r="AR9" s="85"/>
-      <c r="AS9" s="86"/>
-      <c r="AT9" s="87"/>
-      <c r="AU9" s="85"/>
-      <c r="AV9" s="86"/>
-      <c r="AW9" s="87"/>
-      <c r="AX9" s="85"/>
-      <c r="AY9" s="86"/>
-      <c r="AZ9" s="87"/>
-      <c r="BA9" s="103"/>
-      <c r="BB9" s="104"/>
-      <c r="BC9" s="104"/>
-      <c r="BD9" s="104"/>
-      <c r="BE9" s="104"/>
-      <c r="BF9" s="104"/>
-      <c r="BG9" s="104"/>
-      <c r="BH9" s="105"/>
-      <c r="BI9" s="18"/>
-    </row>
-    <row r="10" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A10" s="88">
-        <v>2</v>
-      </c>
-      <c r="B10" s="89"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="130"/>
-      <c r="H10" s="92" t="s">
+      <c r="AY10" s="96"/>
+      <c r="AZ10" s="97"/>
+      <c r="BA10" s="107" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB10" s="134"/>
+      <c r="BC10" s="134"/>
+      <c r="BD10" s="134"/>
+      <c r="BE10" s="134"/>
+      <c r="BF10" s="134"/>
+      <c r="BG10" s="134"/>
+      <c r="BH10" s="135"/>
+      <c r="BI10" s="18"/>
+    </row>
+    <row r="11" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A11" s="76"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="88"/>
+      <c r="T11" s="90"/>
+      <c r="U11" s="87"/>
+      <c r="V11" s="87"/>
+      <c r="W11" s="87"/>
+      <c r="X11" s="87"/>
+      <c r="Y11" s="87"/>
+      <c r="Z11" s="87"/>
+      <c r="AA11" s="87"/>
+      <c r="AB11" s="87"/>
+      <c r="AC11" s="92"/>
+      <c r="AD11" s="93"/>
+      <c r="AE11" s="93"/>
+      <c r="AF11" s="93"/>
+      <c r="AG11" s="93"/>
+      <c r="AH11" s="93"/>
+      <c r="AI11" s="93"/>
+      <c r="AJ11" s="93"/>
+      <c r="AK11" s="93"/>
+      <c r="AL11" s="93"/>
+      <c r="AM11" s="94"/>
+      <c r="AN11" s="98"/>
+      <c r="AO11" s="99"/>
+      <c r="AP11" s="99"/>
+      <c r="AQ11" s="100"/>
+      <c r="AR11" s="98"/>
+      <c r="AS11" s="99"/>
+      <c r="AT11" s="100"/>
+      <c r="AU11" s="98"/>
+      <c r="AV11" s="99"/>
+      <c r="AW11" s="100"/>
+      <c r="AX11" s="98"/>
+      <c r="AY11" s="99"/>
+      <c r="AZ11" s="100"/>
+      <c r="BA11" s="104"/>
+      <c r="BB11" s="165"/>
+      <c r="BC11" s="165"/>
+      <c r="BD11" s="165"/>
+      <c r="BE11" s="165"/>
+      <c r="BF11" s="165"/>
+      <c r="BG11" s="165"/>
+      <c r="BH11" s="166"/>
+      <c r="BI11" s="18"/>
+    </row>
+    <row r="12" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A12" s="74">
+        <v>3</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="94"/>
-      <c r="M10" s="98" t="s">
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="84" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="85"/>
+      <c r="O12" s="85"/>
+      <c r="P12" s="85"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="85"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="78"/>
-      <c r="T10" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="U10" s="74"/>
-      <c r="V10" s="74"/>
-      <c r="W10" s="74"/>
-      <c r="X10" s="74"/>
-      <c r="Y10" s="74"/>
-      <c r="Z10" s="74"/>
-      <c r="AA10" s="74"/>
-      <c r="AB10" s="74"/>
-      <c r="AC10" s="77" t="s">
+      <c r="U12" s="85"/>
+      <c r="V12" s="85"/>
+      <c r="W12" s="85"/>
+      <c r="X12" s="85"/>
+      <c r="Y12" s="85"/>
+      <c r="Z12" s="85"/>
+      <c r="AA12" s="85"/>
+      <c r="AB12" s="85"/>
+      <c r="AC12" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD12" s="85"/>
+      <c r="AE12" s="85"/>
+      <c r="AF12" s="85"/>
+      <c r="AG12" s="85"/>
+      <c r="AH12" s="85"/>
+      <c r="AI12" s="85"/>
+      <c r="AJ12" s="85"/>
+      <c r="AK12" s="85"/>
+      <c r="AL12" s="85"/>
+      <c r="AM12" s="86"/>
+      <c r="AN12" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO12" s="96"/>
+      <c r="AP12" s="96"/>
+      <c r="AQ12" s="97"/>
+      <c r="AR12" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS12" s="96"/>
+      <c r="AT12" s="97"/>
+      <c r="AU12" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="AD10" s="74"/>
-      <c r="AE10" s="74"/>
-      <c r="AF10" s="74"/>
-      <c r="AG10" s="74"/>
-      <c r="AH10" s="74"/>
-      <c r="AI10" s="74"/>
-      <c r="AJ10" s="74"/>
-      <c r="AK10" s="74"/>
-      <c r="AL10" s="74"/>
-      <c r="AM10" s="78"/>
-      <c r="AN10" s="82" t="s">
+      <c r="AV12" s="96"/>
+      <c r="AW12" s="97"/>
+      <c r="AX12" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY12" s="96"/>
+      <c r="AZ12" s="97"/>
+      <c r="BA12" s="107" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB12" s="134"/>
+      <c r="BC12" s="134"/>
+      <c r="BD12" s="134"/>
+      <c r="BE12" s="134"/>
+      <c r="BF12" s="134"/>
+      <c r="BG12" s="134"/>
+      <c r="BH12" s="135"/>
+      <c r="BI12" s="18"/>
+    </row>
+    <row r="13" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A13" s="76"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
+      <c r="S13" s="88"/>
+      <c r="T13" s="90"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="87"/>
+      <c r="W13" s="87"/>
+      <c r="X13" s="87"/>
+      <c r="Y13" s="87"/>
+      <c r="Z13" s="87"/>
+      <c r="AA13" s="87"/>
+      <c r="AB13" s="87"/>
+      <c r="AC13" s="92"/>
+      <c r="AD13" s="93"/>
+      <c r="AE13" s="93"/>
+      <c r="AF13" s="93"/>
+      <c r="AG13" s="93"/>
+      <c r="AH13" s="93"/>
+      <c r="AI13" s="93"/>
+      <c r="AJ13" s="93"/>
+      <c r="AK13" s="93"/>
+      <c r="AL13" s="93"/>
+      <c r="AM13" s="94"/>
+      <c r="AN13" s="98"/>
+      <c r="AO13" s="99"/>
+      <c r="AP13" s="99"/>
+      <c r="AQ13" s="100"/>
+      <c r="AR13" s="98"/>
+      <c r="AS13" s="99"/>
+      <c r="AT13" s="100"/>
+      <c r="AU13" s="98"/>
+      <c r="AV13" s="99"/>
+      <c r="AW13" s="100"/>
+      <c r="AX13" s="98"/>
+      <c r="AY13" s="99"/>
+      <c r="AZ13" s="100"/>
+      <c r="BA13" s="104"/>
+      <c r="BB13" s="165"/>
+      <c r="BC13" s="165"/>
+      <c r="BD13" s="165"/>
+      <c r="BE13" s="165"/>
+      <c r="BF13" s="165"/>
+      <c r="BG13" s="165"/>
+      <c r="BH13" s="166"/>
+      <c r="BI13" s="18"/>
+    </row>
+    <row r="14" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A14" s="74">
+        <v>4</v>
+      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="85"/>
+      <c r="O14" s="85"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="85"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="86"/>
+      <c r="T14" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="U14" s="85"/>
+      <c r="V14" s="85"/>
+      <c r="W14" s="85"/>
+      <c r="X14" s="85"/>
+      <c r="Y14" s="85"/>
+      <c r="Z14" s="85"/>
+      <c r="AA14" s="85"/>
+      <c r="AB14" s="85"/>
+      <c r="AC14" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD14" s="85"/>
+      <c r="AE14" s="85"/>
+      <c r="AF14" s="85"/>
+      <c r="AG14" s="85"/>
+      <c r="AH14" s="85"/>
+      <c r="AI14" s="85"/>
+      <c r="AJ14" s="85"/>
+      <c r="AK14" s="85"/>
+      <c r="AL14" s="85"/>
+      <c r="AM14" s="86"/>
+      <c r="AN14" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="AO10" s="83"/>
-      <c r="AP10" s="83"/>
-      <c r="AQ10" s="84"/>
-      <c r="AR10" s="82" t="s">
+      <c r="AO14" s="96"/>
+      <c r="AP14" s="96"/>
+      <c r="AQ14" s="97"/>
+      <c r="AR14" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="AS10" s="83"/>
-      <c r="AT10" s="84"/>
-      <c r="AU10" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV10" s="83"/>
-      <c r="AW10" s="84"/>
-      <c r="AX10" s="82" t="s">
+      <c r="AS14" s="96"/>
+      <c r="AT14" s="97"/>
+      <c r="AU14" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV14" s="96"/>
+      <c r="AW14" s="97"/>
+      <c r="AX14" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="AY10" s="83"/>
-      <c r="AZ10" s="84"/>
-      <c r="BA10" s="149" t="s">
-        <v>31</v>
-      </c>
-      <c r="BB10" s="150"/>
-      <c r="BC10" s="150"/>
-      <c r="BD10" s="150"/>
-      <c r="BE10" s="150"/>
-      <c r="BF10" s="150"/>
-      <c r="BG10" s="150"/>
-      <c r="BH10" s="151"/>
-      <c r="BI10" s="18"/>
-    </row>
-    <row r="11" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A11" s="90"/>
-      <c r="B11" s="91"/>
-      <c r="C11" s="128"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129"/>
-      <c r="G11" s="130"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="97"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="76"/>
-      <c r="S11" s="99"/>
-      <c r="T11" s="75"/>
-      <c r="U11" s="76"/>
-      <c r="V11" s="76"/>
-      <c r="W11" s="76"/>
-      <c r="X11" s="76"/>
-      <c r="Y11" s="76"/>
-      <c r="Z11" s="76"/>
-      <c r="AA11" s="76"/>
-      <c r="AB11" s="76"/>
-      <c r="AC11" s="79"/>
-      <c r="AD11" s="80"/>
-      <c r="AE11" s="80"/>
-      <c r="AF11" s="80"/>
-      <c r="AG11" s="80"/>
-      <c r="AH11" s="80"/>
-      <c r="AI11" s="80"/>
-      <c r="AJ11" s="80"/>
-      <c r="AK11" s="80"/>
-      <c r="AL11" s="80"/>
-      <c r="AM11" s="81"/>
-      <c r="AN11" s="85"/>
-      <c r="AO11" s="86"/>
-      <c r="AP11" s="86"/>
-      <c r="AQ11" s="87"/>
-      <c r="AR11" s="85"/>
-      <c r="AS11" s="86"/>
-      <c r="AT11" s="87"/>
-      <c r="AU11" s="85"/>
-      <c r="AV11" s="86"/>
-      <c r="AW11" s="87"/>
-      <c r="AX11" s="85"/>
-      <c r="AY11" s="86"/>
-      <c r="AZ11" s="87"/>
-      <c r="BA11" s="100"/>
-      <c r="BB11" s="106"/>
-      <c r="BC11" s="106"/>
-      <c r="BD11" s="106"/>
-      <c r="BE11" s="106"/>
-      <c r="BF11" s="106"/>
-      <c r="BG11" s="106"/>
-      <c r="BH11" s="107"/>
-      <c r="BI11" s="18"/>
-    </row>
-    <row r="12" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A12" s="88">
-        <v>3</v>
-      </c>
-      <c r="B12" s="89"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="129"/>
-      <c r="E12" s="129"/>
-      <c r="F12" s="129"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="92" t="s">
+      <c r="AY14" s="96"/>
+      <c r="AZ14" s="97"/>
+      <c r="BA14" s="104" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB14" s="105"/>
+      <c r="BC14" s="105"/>
+      <c r="BD14" s="105"/>
+      <c r="BE14" s="105"/>
+      <c r="BF14" s="105"/>
+      <c r="BG14" s="105"/>
+      <c r="BH14" s="106"/>
+      <c r="BI14" s="18"/>
+    </row>
+    <row r="15" spans="1:61" s="58" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A15" s="76"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="87"/>
+      <c r="R15" s="87"/>
+      <c r="S15" s="88"/>
+      <c r="T15" s="90"/>
+      <c r="U15" s="87"/>
+      <c r="V15" s="87"/>
+      <c r="W15" s="87"/>
+      <c r="X15" s="87"/>
+      <c r="Y15" s="87"/>
+      <c r="Z15" s="87"/>
+      <c r="AA15" s="87"/>
+      <c r="AB15" s="87"/>
+      <c r="AC15" s="92"/>
+      <c r="AD15" s="93"/>
+      <c r="AE15" s="93"/>
+      <c r="AF15" s="93"/>
+      <c r="AG15" s="93"/>
+      <c r="AH15" s="93"/>
+      <c r="AI15" s="93"/>
+      <c r="AJ15" s="93"/>
+      <c r="AK15" s="93"/>
+      <c r="AL15" s="93"/>
+      <c r="AM15" s="94"/>
+      <c r="AN15" s="98"/>
+      <c r="AO15" s="99"/>
+      <c r="AP15" s="99"/>
+      <c r="AQ15" s="100"/>
+      <c r="AR15" s="98"/>
+      <c r="AS15" s="99"/>
+      <c r="AT15" s="100"/>
+      <c r="AU15" s="98"/>
+      <c r="AV15" s="99"/>
+      <c r="AW15" s="100"/>
+      <c r="AX15" s="98"/>
+      <c r="AY15" s="99"/>
+      <c r="AZ15" s="100"/>
+      <c r="BA15" s="104"/>
+      <c r="BB15" s="105"/>
+      <c r="BC15" s="105"/>
+      <c r="BD15" s="105"/>
+      <c r="BE15" s="105"/>
+      <c r="BF15" s="105"/>
+      <c r="BG15" s="105"/>
+      <c r="BH15" s="106"/>
+      <c r="BI15" s="57"/>
+    </row>
+    <row r="16" spans="1:61" s="60" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A16" s="74">
+        <v>5</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="94"/>
-      <c r="M12" s="98" t="s">
-        <v>47</v>
-      </c>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="78"/>
-      <c r="T12" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="U12" s="74"/>
-      <c r="V12" s="74"/>
-      <c r="W12" s="74"/>
-      <c r="X12" s="74"/>
-      <c r="Y12" s="74"/>
-      <c r="Z12" s="74"/>
-      <c r="AA12" s="74"/>
-      <c r="AB12" s="74"/>
-      <c r="AC12" s="77" t="s">
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="84" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="85"/>
+      <c r="O16" s="85"/>
+      <c r="P16" s="85"/>
+      <c r="Q16" s="85"/>
+      <c r="R16" s="85"/>
+      <c r="S16" s="86"/>
+      <c r="T16" s="89" t="s">
+        <v>44</v>
+      </c>
+      <c r="U16" s="85"/>
+      <c r="V16" s="85"/>
+      <c r="W16" s="85"/>
+      <c r="X16" s="85"/>
+      <c r="Y16" s="85"/>
+      <c r="Z16" s="85"/>
+      <c r="AA16" s="85"/>
+      <c r="AB16" s="85"/>
+      <c r="AC16" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD16" s="85"/>
+      <c r="AE16" s="85"/>
+      <c r="AF16" s="85"/>
+      <c r="AG16" s="85"/>
+      <c r="AH16" s="85"/>
+      <c r="AI16" s="85"/>
+      <c r="AJ16" s="85"/>
+      <c r="AK16" s="85"/>
+      <c r="AL16" s="85"/>
+      <c r="AM16" s="86"/>
+      <c r="AN16" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO16" s="96"/>
+      <c r="AP16" s="96"/>
+      <c r="AQ16" s="97"/>
+      <c r="AR16" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS16" s="96"/>
+      <c r="AT16" s="97"/>
+      <c r="AU16" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="AD12" s="74"/>
-      <c r="AE12" s="74"/>
-      <c r="AF12" s="74"/>
-      <c r="AG12" s="74"/>
-      <c r="AH12" s="74"/>
-      <c r="AI12" s="74"/>
-      <c r="AJ12" s="74"/>
-      <c r="AK12" s="74"/>
-      <c r="AL12" s="74"/>
-      <c r="AM12" s="78"/>
-      <c r="AN12" s="82" t="s">
+      <c r="AV16" s="96"/>
+      <c r="AW16" s="97"/>
+      <c r="AX16" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY16" s="96"/>
+      <c r="AZ16" s="97"/>
+      <c r="BA16" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB16" s="105"/>
+      <c r="BC16" s="105"/>
+      <c r="BD16" s="105"/>
+      <c r="BE16" s="105"/>
+      <c r="BF16" s="105"/>
+      <c r="BG16" s="105"/>
+      <c r="BH16" s="106"/>
+      <c r="BI16" s="59"/>
+    </row>
+    <row r="17" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A17" s="76"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="103"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="87"/>
+      <c r="R17" s="87"/>
+      <c r="S17" s="88"/>
+      <c r="T17" s="90"/>
+      <c r="U17" s="87"/>
+      <c r="V17" s="87"/>
+      <c r="W17" s="87"/>
+      <c r="X17" s="87"/>
+      <c r="Y17" s="87"/>
+      <c r="Z17" s="87"/>
+      <c r="AA17" s="87"/>
+      <c r="AB17" s="87"/>
+      <c r="AC17" s="92"/>
+      <c r="AD17" s="93"/>
+      <c r="AE17" s="93"/>
+      <c r="AF17" s="93"/>
+      <c r="AG17" s="93"/>
+      <c r="AH17" s="93"/>
+      <c r="AI17" s="93"/>
+      <c r="AJ17" s="93"/>
+      <c r="AK17" s="93"/>
+      <c r="AL17" s="93"/>
+      <c r="AM17" s="94"/>
+      <c r="AN17" s="98"/>
+      <c r="AO17" s="99"/>
+      <c r="AP17" s="99"/>
+      <c r="AQ17" s="100"/>
+      <c r="AR17" s="98"/>
+      <c r="AS17" s="99"/>
+      <c r="AT17" s="100"/>
+      <c r="AU17" s="98"/>
+      <c r="AV17" s="99"/>
+      <c r="AW17" s="100"/>
+      <c r="AX17" s="98"/>
+      <c r="AY17" s="99"/>
+      <c r="AZ17" s="100"/>
+      <c r="BA17" s="107"/>
+      <c r="BB17" s="108"/>
+      <c r="BC17" s="108"/>
+      <c r="BD17" s="108"/>
+      <c r="BE17" s="108"/>
+      <c r="BF17" s="108"/>
+      <c r="BG17" s="108"/>
+      <c r="BH17" s="109"/>
+      <c r="BI17" s="18"/>
+    </row>
+    <row r="18" spans="1:61" s="60" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A18" s="74">
+        <v>6</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" s="85"/>
+      <c r="O18" s="85"/>
+      <c r="P18" s="85"/>
+      <c r="Q18" s="85"/>
+      <c r="R18" s="85"/>
+      <c r="S18" s="86"/>
+      <c r="T18" s="89" t="s">
+        <v>40</v>
+      </c>
+      <c r="U18" s="85"/>
+      <c r="V18" s="85"/>
+      <c r="W18" s="85"/>
+      <c r="X18" s="85"/>
+      <c r="Y18" s="85"/>
+      <c r="Z18" s="85"/>
+      <c r="AA18" s="85"/>
+      <c r="AB18" s="85"/>
+      <c r="AC18" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD18" s="85"/>
+      <c r="AE18" s="85"/>
+      <c r="AF18" s="85"/>
+      <c r="AG18" s="85"/>
+      <c r="AH18" s="85"/>
+      <c r="AI18" s="85"/>
+      <c r="AJ18" s="85"/>
+      <c r="AK18" s="85"/>
+      <c r="AL18" s="85"/>
+      <c r="AM18" s="86"/>
+      <c r="AN18" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="AO12" s="83"/>
-      <c r="AP12" s="83"/>
-      <c r="AQ12" s="84"/>
-      <c r="AR12" s="82" t="s">
+      <c r="AO18" s="96"/>
+      <c r="AP18" s="96"/>
+      <c r="AQ18" s="97"/>
+      <c r="AR18" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="AS12" s="83"/>
-      <c r="AT12" s="84"/>
-      <c r="AU12" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV12" s="83"/>
-      <c r="AW12" s="84"/>
-      <c r="AX12" s="82" t="s">
+      <c r="AS18" s="96"/>
+      <c r="AT18" s="97"/>
+      <c r="AU18" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV18" s="96"/>
+      <c r="AW18" s="97"/>
+      <c r="AX18" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="AY12" s="83"/>
-      <c r="AZ12" s="84"/>
-      <c r="BA12" s="149" t="s">
-        <v>33</v>
-      </c>
-      <c r="BB12" s="150"/>
-      <c r="BC12" s="150"/>
-      <c r="BD12" s="150"/>
-      <c r="BE12" s="150"/>
-      <c r="BF12" s="150"/>
-      <c r="BG12" s="150"/>
-      <c r="BH12" s="151"/>
-      <c r="BI12" s="18"/>
-    </row>
-    <row r="13" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A13" s="90"/>
-      <c r="B13" s="91"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
-      <c r="G13" s="130"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="130"/>
-      <c r="M13" s="76"/>
-      <c r="N13" s="76"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="99"/>
-      <c r="T13" s="75"/>
-      <c r="U13" s="76"/>
-      <c r="V13" s="76"/>
-      <c r="W13" s="76"/>
-      <c r="X13" s="76"/>
-      <c r="Y13" s="76"/>
-      <c r="Z13" s="76"/>
-      <c r="AA13" s="76"/>
-      <c r="AB13" s="76"/>
-      <c r="AC13" s="79"/>
-      <c r="AD13" s="80"/>
-      <c r="AE13" s="80"/>
-      <c r="AF13" s="80"/>
-      <c r="AG13" s="80"/>
-      <c r="AH13" s="80"/>
-      <c r="AI13" s="80"/>
-      <c r="AJ13" s="80"/>
-      <c r="AK13" s="80"/>
-      <c r="AL13" s="80"/>
-      <c r="AM13" s="81"/>
-      <c r="AN13" s="85"/>
-      <c r="AO13" s="86"/>
-      <c r="AP13" s="86"/>
-      <c r="AQ13" s="87"/>
-      <c r="AR13" s="85"/>
-      <c r="AS13" s="86"/>
-      <c r="AT13" s="87"/>
-      <c r="AU13" s="85"/>
-      <c r="AV13" s="86"/>
-      <c r="AW13" s="87"/>
-      <c r="AX13" s="85"/>
-      <c r="AY13" s="86"/>
-      <c r="AZ13" s="87"/>
-      <c r="BA13" s="100"/>
-      <c r="BB13" s="106"/>
-      <c r="BC13" s="106"/>
-      <c r="BD13" s="106"/>
-      <c r="BE13" s="106"/>
-      <c r="BF13" s="106"/>
-      <c r="BG13" s="106"/>
-      <c r="BH13" s="107"/>
-      <c r="BI13" s="18"/>
-    </row>
-    <row r="14" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A14" s="88">
-        <v>4</v>
-      </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="128"/>
-      <c r="D14" s="129"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="129"/>
-      <c r="G14" s="130"/>
-      <c r="H14" s="92" t="s">
+      <c r="AY18" s="96"/>
+      <c r="AZ18" s="97"/>
+      <c r="BA18" s="104" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB18" s="105"/>
+      <c r="BC18" s="105"/>
+      <c r="BD18" s="105"/>
+      <c r="BE18" s="105"/>
+      <c r="BF18" s="105"/>
+      <c r="BG18" s="105"/>
+      <c r="BH18" s="106"/>
+      <c r="BI18" s="59"/>
+    </row>
+    <row r="19" spans="1:61" s="58" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A19" s="76"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="87"/>
+      <c r="R19" s="87"/>
+      <c r="S19" s="88"/>
+      <c r="T19" s="90"/>
+      <c r="U19" s="87"/>
+      <c r="V19" s="87"/>
+      <c r="W19" s="87"/>
+      <c r="X19" s="87"/>
+      <c r="Y19" s="87"/>
+      <c r="Z19" s="87"/>
+      <c r="AA19" s="87"/>
+      <c r="AB19" s="87"/>
+      <c r="AC19" s="92"/>
+      <c r="AD19" s="93"/>
+      <c r="AE19" s="93"/>
+      <c r="AF19" s="93"/>
+      <c r="AG19" s="93"/>
+      <c r="AH19" s="93"/>
+      <c r="AI19" s="93"/>
+      <c r="AJ19" s="93"/>
+      <c r="AK19" s="93"/>
+      <c r="AL19" s="93"/>
+      <c r="AM19" s="94"/>
+      <c r="AN19" s="98"/>
+      <c r="AO19" s="99"/>
+      <c r="AP19" s="99"/>
+      <c r="AQ19" s="100"/>
+      <c r="AR19" s="98"/>
+      <c r="AS19" s="99"/>
+      <c r="AT19" s="100"/>
+      <c r="AU19" s="98"/>
+      <c r="AV19" s="99"/>
+      <c r="AW19" s="100"/>
+      <c r="AX19" s="98"/>
+      <c r="AY19" s="99"/>
+      <c r="AZ19" s="100"/>
+      <c r="BA19" s="104"/>
+      <c r="BB19" s="105"/>
+      <c r="BC19" s="105"/>
+      <c r="BD19" s="105"/>
+      <c r="BE19" s="105"/>
+      <c r="BF19" s="105"/>
+      <c r="BG19" s="105"/>
+      <c r="BH19" s="106"/>
+      <c r="BI19" s="57"/>
+    </row>
+    <row r="20" spans="1:61" s="60" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A20" s="74">
+        <v>7</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="94"/>
-      <c r="M14" s="98" t="s">
-        <v>48</v>
-      </c>
-      <c r="N14" s="74"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="74"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="78"/>
-      <c r="T14" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="U14" s="74"/>
-      <c r="V14" s="74"/>
-      <c r="W14" s="74"/>
-      <c r="X14" s="74"/>
-      <c r="Y14" s="74"/>
-      <c r="Z14" s="74"/>
-      <c r="AA14" s="74"/>
-      <c r="AB14" s="74"/>
-      <c r="AC14" s="77" t="s">
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="80"/>
+      <c r="M20" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="85"/>
+      <c r="Q20" s="85"/>
+      <c r="R20" s="85"/>
+      <c r="S20" s="86"/>
+      <c r="T20" s="89" t="s">
+        <v>40</v>
+      </c>
+      <c r="U20" s="85"/>
+      <c r="V20" s="85"/>
+      <c r="W20" s="85"/>
+      <c r="X20" s="85"/>
+      <c r="Y20" s="85"/>
+      <c r="Z20" s="85"/>
+      <c r="AA20" s="85"/>
+      <c r="AB20" s="85"/>
+      <c r="AC20" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD20" s="85"/>
+      <c r="AE20" s="85"/>
+      <c r="AF20" s="85"/>
+      <c r="AG20" s="85"/>
+      <c r="AH20" s="85"/>
+      <c r="AI20" s="85"/>
+      <c r="AJ20" s="85"/>
+      <c r="AK20" s="85"/>
+      <c r="AL20" s="85"/>
+      <c r="AM20" s="86"/>
+      <c r="AN20" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO20" s="96"/>
+      <c r="AP20" s="96"/>
+      <c r="AQ20" s="97"/>
+      <c r="AR20" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS20" s="96"/>
+      <c r="AT20" s="97"/>
+      <c r="AU20" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="AD14" s="74"/>
-      <c r="AE14" s="74"/>
-      <c r="AF14" s="74"/>
-      <c r="AG14" s="74"/>
-      <c r="AH14" s="74"/>
-      <c r="AI14" s="74"/>
-      <c r="AJ14" s="74"/>
-      <c r="AK14" s="74"/>
-      <c r="AL14" s="74"/>
-      <c r="AM14" s="78"/>
-      <c r="AN14" s="82" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO14" s="83"/>
-      <c r="AP14" s="83"/>
-      <c r="AQ14" s="84"/>
-      <c r="AR14" s="82" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS14" s="83"/>
-      <c r="AT14" s="84"/>
-      <c r="AU14" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV14" s="83"/>
-      <c r="AW14" s="84"/>
-      <c r="AX14" s="82" t="s">
+      <c r="AV20" s="96"/>
+      <c r="AW20" s="97"/>
+      <c r="AX20" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="AY14" s="83"/>
-      <c r="AZ14" s="84"/>
-      <c r="BA14" s="100" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB14" s="101"/>
-      <c r="BC14" s="101"/>
-      <c r="BD14" s="101"/>
-      <c r="BE14" s="101"/>
-      <c r="BF14" s="101"/>
-      <c r="BG14" s="101"/>
-      <c r="BH14" s="102"/>
-      <c r="BI14" s="18"/>
-    </row>
-    <row r="15" spans="1:61" s="58" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A15" s="90"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
-      <c r="G15" s="130"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="96"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="96"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="99"/>
-      <c r="T15" s="75"/>
-      <c r="U15" s="76"/>
-      <c r="V15" s="76"/>
-      <c r="W15" s="76"/>
-      <c r="X15" s="76"/>
-      <c r="Y15" s="76"/>
-      <c r="Z15" s="76"/>
-      <c r="AA15" s="76"/>
-      <c r="AB15" s="76"/>
-      <c r="AC15" s="79"/>
-      <c r="AD15" s="80"/>
-      <c r="AE15" s="80"/>
-      <c r="AF15" s="80"/>
-      <c r="AG15" s="80"/>
-      <c r="AH15" s="80"/>
-      <c r="AI15" s="80"/>
-      <c r="AJ15" s="80"/>
-      <c r="AK15" s="80"/>
-      <c r="AL15" s="80"/>
-      <c r="AM15" s="81"/>
-      <c r="AN15" s="85"/>
-      <c r="AO15" s="86"/>
-      <c r="AP15" s="86"/>
-      <c r="AQ15" s="87"/>
-      <c r="AR15" s="85"/>
-      <c r="AS15" s="86"/>
-      <c r="AT15" s="87"/>
-      <c r="AU15" s="85"/>
-      <c r="AV15" s="86"/>
-      <c r="AW15" s="87"/>
-      <c r="AX15" s="85"/>
-      <c r="AY15" s="86"/>
-      <c r="AZ15" s="87"/>
-      <c r="BA15" s="100"/>
-      <c r="BB15" s="101"/>
-      <c r="BC15" s="101"/>
-      <c r="BD15" s="101"/>
-      <c r="BE15" s="101"/>
-      <c r="BF15" s="101"/>
-      <c r="BG15" s="101"/>
-      <c r="BH15" s="102"/>
-      <c r="BI15" s="57"/>
-    </row>
-    <row r="16" spans="1:61" s="60" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A16" s="88">
-        <v>5</v>
-      </c>
-      <c r="B16" s="89"/>
-      <c r="C16" s="128"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
-      <c r="F16" s="129"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="92" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="94"/>
-      <c r="M16" s="98" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="78"/>
-      <c r="T16" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
-      <c r="Z16" s="74"/>
-      <c r="AA16" s="74"/>
-      <c r="AB16" s="74"/>
-      <c r="AC16" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD16" s="74"/>
-      <c r="AE16" s="74"/>
-      <c r="AF16" s="74"/>
-      <c r="AG16" s="74"/>
-      <c r="AH16" s="74"/>
-      <c r="AI16" s="74"/>
-      <c r="AJ16" s="74"/>
-      <c r="AK16" s="74"/>
-      <c r="AL16" s="74"/>
-      <c r="AM16" s="78"/>
-      <c r="AN16" s="82" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO16" s="83"/>
-      <c r="AP16" s="83"/>
-      <c r="AQ16" s="84"/>
-      <c r="AR16" s="82" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS16" s="83"/>
-      <c r="AT16" s="84"/>
-      <c r="AU16" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV16" s="83"/>
-      <c r="AW16" s="84"/>
-      <c r="AX16" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY16" s="83"/>
-      <c r="AZ16" s="84"/>
-      <c r="BA16" s="100" t="s">
-        <v>34</v>
-      </c>
-      <c r="BB16" s="101"/>
-      <c r="BC16" s="101"/>
-      <c r="BD16" s="101"/>
-      <c r="BE16" s="101"/>
-      <c r="BF16" s="101"/>
-      <c r="BG16" s="101"/>
-      <c r="BH16" s="102"/>
-      <c r="BI16" s="59"/>
-    </row>
-    <row r="17" spans="1:61" s="12" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A17" s="90"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="129"/>
-      <c r="G17" s="130"/>
-      <c r="H17" s="128"/>
-      <c r="I17" s="129"/>
-      <c r="J17" s="129"/>
-      <c r="K17" s="129"/>
-      <c r="L17" s="130"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="99"/>
-      <c r="T17" s="75"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="79"/>
-      <c r="AD17" s="80"/>
-      <c r="AE17" s="80"/>
-      <c r="AF17" s="80"/>
-      <c r="AG17" s="80"/>
-      <c r="AH17" s="80"/>
-      <c r="AI17" s="80"/>
-      <c r="AJ17" s="80"/>
-      <c r="AK17" s="80"/>
-      <c r="AL17" s="80"/>
-      <c r="AM17" s="81"/>
-      <c r="AN17" s="85"/>
-      <c r="AO17" s="86"/>
-      <c r="AP17" s="86"/>
-      <c r="AQ17" s="87"/>
-      <c r="AR17" s="85"/>
-      <c r="AS17" s="86"/>
-      <c r="AT17" s="87"/>
-      <c r="AU17" s="85"/>
-      <c r="AV17" s="86"/>
-      <c r="AW17" s="87"/>
-      <c r="AX17" s="85"/>
-      <c r="AY17" s="86"/>
-      <c r="AZ17" s="87"/>
-      <c r="BA17" s="149"/>
-      <c r="BB17" s="164"/>
-      <c r="BC17" s="164"/>
-      <c r="BD17" s="164"/>
-      <c r="BE17" s="164"/>
-      <c r="BF17" s="164"/>
-      <c r="BG17" s="164"/>
-      <c r="BH17" s="165"/>
-      <c r="BI17" s="18"/>
-    </row>
-    <row r="18" spans="1:61" s="60" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A18" s="88">
-        <v>6</v>
-      </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="128"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="129"/>
-      <c r="F18" s="129"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="92" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="N18" s="74"/>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-      <c r="S18" s="78"/>
-      <c r="T18" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74"/>
-      <c r="X18" s="74"/>
-      <c r="Y18" s="74"/>
-      <c r="Z18" s="74"/>
-      <c r="AA18" s="74"/>
-      <c r="AB18" s="74"/>
-      <c r="AC18" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD18" s="74"/>
-      <c r="AE18" s="74"/>
-      <c r="AF18" s="74"/>
-      <c r="AG18" s="74"/>
-      <c r="AH18" s="74"/>
-      <c r="AI18" s="74"/>
-      <c r="AJ18" s="74"/>
-      <c r="AK18" s="74"/>
-      <c r="AL18" s="74"/>
-      <c r="AM18" s="78"/>
-      <c r="AN18" s="82" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO18" s="83"/>
-      <c r="AP18" s="83"/>
-      <c r="AQ18" s="84"/>
-      <c r="AR18" s="82" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS18" s="83"/>
-      <c r="AT18" s="84"/>
-      <c r="AU18" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV18" s="83"/>
-      <c r="AW18" s="84"/>
-      <c r="AX18" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY18" s="83"/>
-      <c r="AZ18" s="84"/>
-      <c r="BA18" s="100" t="s">
-        <v>37</v>
-      </c>
-      <c r="BB18" s="101"/>
-      <c r="BC18" s="101"/>
-      <c r="BD18" s="101"/>
-      <c r="BE18" s="101"/>
-      <c r="BF18" s="101"/>
-      <c r="BG18" s="101"/>
-      <c r="BH18" s="102"/>
-      <c r="BI18" s="59"/>
-    </row>
-    <row r="19" spans="1:61" s="58" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A19" s="90"/>
-      <c r="B19" s="91"/>
-      <c r="C19" s="128"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="129"/>
-      <c r="G19" s="130"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="97"/>
-      <c r="M19" s="76"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="76"/>
-      <c r="S19" s="99"/>
-      <c r="T19" s="75"/>
-      <c r="U19" s="76"/>
-      <c r="V19" s="76"/>
-      <c r="W19" s="76"/>
-      <c r="X19" s="76"/>
-      <c r="Y19" s="76"/>
-      <c r="Z19" s="76"/>
-      <c r="AA19" s="76"/>
-      <c r="AB19" s="76"/>
-      <c r="AC19" s="79"/>
-      <c r="AD19" s="80"/>
-      <c r="AE19" s="80"/>
-      <c r="AF19" s="80"/>
-      <c r="AG19" s="80"/>
-      <c r="AH19" s="80"/>
-      <c r="AI19" s="80"/>
-      <c r="AJ19" s="80"/>
-      <c r="AK19" s="80"/>
-      <c r="AL19" s="80"/>
-      <c r="AM19" s="81"/>
-      <c r="AN19" s="85"/>
-      <c r="AO19" s="86"/>
-      <c r="AP19" s="86"/>
-      <c r="AQ19" s="87"/>
-      <c r="AR19" s="85"/>
-      <c r="AS19" s="86"/>
-      <c r="AT19" s="87"/>
-      <c r="AU19" s="85"/>
-      <c r="AV19" s="86"/>
-      <c r="AW19" s="87"/>
-      <c r="AX19" s="85"/>
-      <c r="AY19" s="86"/>
-      <c r="AZ19" s="87"/>
-      <c r="BA19" s="100"/>
-      <c r="BB19" s="101"/>
-      <c r="BC19" s="101"/>
-      <c r="BD19" s="101"/>
-      <c r="BE19" s="101"/>
-      <c r="BF19" s="101"/>
-      <c r="BG19" s="101"/>
-      <c r="BH19" s="102"/>
-      <c r="BI19" s="57"/>
-    </row>
-    <row r="20" spans="1:61" s="60" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A20" s="88">
-        <v>7</v>
-      </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="92" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="93"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="94"/>
-      <c r="M20" s="98" t="s">
-        <v>52</v>
-      </c>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74"/>
-      <c r="S20" s="78"/>
-      <c r="T20" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="U20" s="74"/>
-      <c r="V20" s="74"/>
-      <c r="W20" s="74"/>
-      <c r="X20" s="74"/>
-      <c r="Y20" s="74"/>
-      <c r="Z20" s="74"/>
-      <c r="AA20" s="74"/>
-      <c r="AB20" s="74"/>
-      <c r="AC20" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD20" s="74"/>
-      <c r="AE20" s="74"/>
-      <c r="AF20" s="74"/>
-      <c r="AG20" s="74"/>
-      <c r="AH20" s="74"/>
-      <c r="AI20" s="74"/>
-      <c r="AJ20" s="74"/>
-      <c r="AK20" s="74"/>
-      <c r="AL20" s="74"/>
-      <c r="AM20" s="78"/>
-      <c r="AN20" s="82" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO20" s="83"/>
-      <c r="AP20" s="83"/>
-      <c r="AQ20" s="84"/>
-      <c r="AR20" s="82" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS20" s="83"/>
-      <c r="AT20" s="84"/>
-      <c r="AU20" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV20" s="83"/>
-      <c r="AW20" s="84"/>
-      <c r="AX20" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY20" s="83"/>
-      <c r="AZ20" s="84"/>
-      <c r="BA20" s="100" t="s">
+      <c r="AY20" s="96"/>
+      <c r="AZ20" s="97"/>
+      <c r="BA20" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="BB20" s="101"/>
-      <c r="BC20" s="101"/>
-      <c r="BD20" s="101"/>
-      <c r="BE20" s="101"/>
-      <c r="BF20" s="101"/>
-      <c r="BG20" s="101"/>
-      <c r="BH20" s="102"/>
+      <c r="BB20" s="105"/>
+      <c r="BC20" s="105"/>
+      <c r="BD20" s="105"/>
+      <c r="BE20" s="105"/>
+      <c r="BF20" s="105"/>
+      <c r="BG20" s="105"/>
+      <c r="BH20" s="106"/>
       <c r="BI20" s="59"/>
     </row>
     <row r="21" spans="1:61" s="58" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A21" s="90"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="128"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="96"/>
-      <c r="J21" s="96"/>
-      <c r="K21" s="96"/>
-      <c r="L21" s="97"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="76"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="76"/>
-      <c r="Q21" s="76"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="99"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="76"/>
-      <c r="V21" s="76"/>
-      <c r="W21" s="76"/>
-      <c r="X21" s="76"/>
-      <c r="Y21" s="76"/>
-      <c r="Z21" s="76"/>
-      <c r="AA21" s="76"/>
-      <c r="AB21" s="76"/>
-      <c r="AC21" s="79"/>
-      <c r="AD21" s="80"/>
-      <c r="AE21" s="80"/>
-      <c r="AF21" s="80"/>
-      <c r="AG21" s="80"/>
-      <c r="AH21" s="80"/>
-      <c r="AI21" s="80"/>
-      <c r="AJ21" s="80"/>
-      <c r="AK21" s="80"/>
-      <c r="AL21" s="80"/>
-      <c r="AM21" s="81"/>
-      <c r="AN21" s="85"/>
-      <c r="AO21" s="86"/>
-      <c r="AP21" s="86"/>
-      <c r="AQ21" s="87"/>
-      <c r="AR21" s="85"/>
-      <c r="AS21" s="86"/>
-      <c r="AT21" s="87"/>
-      <c r="AU21" s="85"/>
-      <c r="AV21" s="86"/>
-      <c r="AW21" s="87"/>
-      <c r="AX21" s="85"/>
-      <c r="AY21" s="86"/>
-      <c r="AZ21" s="87"/>
-      <c r="BA21" s="100"/>
-      <c r="BB21" s="101"/>
-      <c r="BC21" s="101"/>
-      <c r="BD21" s="101"/>
-      <c r="BE21" s="101"/>
-      <c r="BF21" s="101"/>
-      <c r="BG21" s="101"/>
-      <c r="BH21" s="102"/>
+      <c r="A21" s="76"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="87"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="87"/>
+      <c r="R21" s="87"/>
+      <c r="S21" s="88"/>
+      <c r="T21" s="90"/>
+      <c r="U21" s="87"/>
+      <c r="V21" s="87"/>
+      <c r="W21" s="87"/>
+      <c r="X21" s="87"/>
+      <c r="Y21" s="87"/>
+      <c r="Z21" s="87"/>
+      <c r="AA21" s="87"/>
+      <c r="AB21" s="87"/>
+      <c r="AC21" s="92"/>
+      <c r="AD21" s="93"/>
+      <c r="AE21" s="93"/>
+      <c r="AF21" s="93"/>
+      <c r="AG21" s="93"/>
+      <c r="AH21" s="93"/>
+      <c r="AI21" s="93"/>
+      <c r="AJ21" s="93"/>
+      <c r="AK21" s="93"/>
+      <c r="AL21" s="93"/>
+      <c r="AM21" s="94"/>
+      <c r="AN21" s="98"/>
+      <c r="AO21" s="99"/>
+      <c r="AP21" s="99"/>
+      <c r="AQ21" s="100"/>
+      <c r="AR21" s="98"/>
+      <c r="AS21" s="99"/>
+      <c r="AT21" s="100"/>
+      <c r="AU21" s="98"/>
+      <c r="AV21" s="99"/>
+      <c r="AW21" s="100"/>
+      <c r="AX21" s="98"/>
+      <c r="AY21" s="99"/>
+      <c r="AZ21" s="100"/>
+      <c r="BA21" s="104"/>
+      <c r="BB21" s="105"/>
+      <c r="BC21" s="105"/>
+      <c r="BD21" s="105"/>
+      <c r="BE21" s="105"/>
+      <c r="BF21" s="105"/>
+      <c r="BG21" s="105"/>
+      <c r="BH21" s="106"/>
       <c r="BI21" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="H20:L21"/>
-    <mergeCell ref="M20:S21"/>
-    <mergeCell ref="T20:AB21"/>
-    <mergeCell ref="AC20:AM21"/>
-    <mergeCell ref="AN20:AQ21"/>
-    <mergeCell ref="AR20:AT21"/>
-    <mergeCell ref="AU20:AW21"/>
-    <mergeCell ref="C8:G21"/>
-    <mergeCell ref="AN18:AQ19"/>
-    <mergeCell ref="AR18:AT19"/>
-    <mergeCell ref="AU18:AW19"/>
-    <mergeCell ref="AX18:AZ19"/>
-    <mergeCell ref="BA18:BH18"/>
-    <mergeCell ref="BA19:BH19"/>
-    <mergeCell ref="AX20:AZ21"/>
-    <mergeCell ref="BA20:BH20"/>
-    <mergeCell ref="BA21:BH21"/>
-    <mergeCell ref="AU16:AW17"/>
-    <mergeCell ref="AX14:AZ15"/>
-    <mergeCell ref="AX16:AZ17"/>
-    <mergeCell ref="BA16:BH16"/>
-    <mergeCell ref="BA17:BH17"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="H14:L15"/>
-    <mergeCell ref="M14:S15"/>
-    <mergeCell ref="T14:AB15"/>
-    <mergeCell ref="AC14:AM15"/>
-    <mergeCell ref="H16:L17"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="M16:S17"/>
-    <mergeCell ref="T16:AB17"/>
-    <mergeCell ref="AC16:AM17"/>
-    <mergeCell ref="BA14:BH14"/>
-    <mergeCell ref="BA15:BH15"/>
-    <mergeCell ref="AN14:AQ15"/>
-    <mergeCell ref="AN16:AQ17"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="H10:L11"/>
+    <mergeCell ref="M10:S11"/>
+    <mergeCell ref="T10:AB11"/>
+    <mergeCell ref="BA8:BH8"/>
+    <mergeCell ref="AX8:AZ9"/>
+    <mergeCell ref="AU8:AW9"/>
+    <mergeCell ref="AR8:AT9"/>
+    <mergeCell ref="AN8:AQ9"/>
+    <mergeCell ref="BA9:BH9"/>
+    <mergeCell ref="AC8:AM9"/>
+    <mergeCell ref="AC10:AM11"/>
+    <mergeCell ref="AR10:AT11"/>
+    <mergeCell ref="AU10:AW11"/>
+    <mergeCell ref="AX10:AZ11"/>
+    <mergeCell ref="BA11:BH11"/>
+    <mergeCell ref="AN10:AQ11"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="H18:L19"/>
+    <mergeCell ref="M18:S19"/>
+    <mergeCell ref="T18:AB19"/>
+    <mergeCell ref="AC18:AM19"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="M12:S13"/>
+    <mergeCell ref="T12:AB13"/>
+    <mergeCell ref="AC12:AM13"/>
+    <mergeCell ref="A3:G4"/>
+    <mergeCell ref="H3:AI4"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="T6:AB7"/>
+    <mergeCell ref="AC6:AM7"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="H8:L9"/>
+    <mergeCell ref="M8:S9"/>
+    <mergeCell ref="T8:AB9"/>
+    <mergeCell ref="AJ3:AM3"/>
+    <mergeCell ref="BA10:BH10"/>
+    <mergeCell ref="BA12:BH12"/>
+    <mergeCell ref="C6:S6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="M7:S7"/>
+    <mergeCell ref="AR6:AT7"/>
+    <mergeCell ref="AU6:AW7"/>
+    <mergeCell ref="AX6:AZ7"/>
+    <mergeCell ref="AN6:AQ7"/>
+    <mergeCell ref="BA6:BH7"/>
+    <mergeCell ref="AR12:AT13"/>
+    <mergeCell ref="AU12:AW13"/>
+    <mergeCell ref="AX12:AZ13"/>
+    <mergeCell ref="AN12:AQ13"/>
+    <mergeCell ref="BA13:BH13"/>
     <mergeCell ref="AR14:AT15"/>
     <mergeCell ref="AR16:AT17"/>
     <mergeCell ref="AU14:AW15"/>
@@ -6562,59 +6576,43 @@
     <mergeCell ref="AN4:AV4"/>
     <mergeCell ref="AW4:AZ4"/>
     <mergeCell ref="BA4:BH4"/>
-    <mergeCell ref="BA10:BH10"/>
-    <mergeCell ref="BA12:BH12"/>
-    <mergeCell ref="C6:S6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="M7:S7"/>
-    <mergeCell ref="AR6:AT7"/>
-    <mergeCell ref="AU6:AW7"/>
-    <mergeCell ref="AX6:AZ7"/>
-    <mergeCell ref="AN6:AQ7"/>
-    <mergeCell ref="BA6:BH7"/>
-    <mergeCell ref="A3:G4"/>
-    <mergeCell ref="H3:AI4"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="T6:AB7"/>
-    <mergeCell ref="AC6:AM7"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="H8:L9"/>
-    <mergeCell ref="M8:S9"/>
-    <mergeCell ref="T8:AB9"/>
-    <mergeCell ref="AJ3:AM3"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="H18:L19"/>
-    <mergeCell ref="M18:S19"/>
-    <mergeCell ref="T18:AB19"/>
-    <mergeCell ref="AC18:AM19"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="H12:L13"/>
-    <mergeCell ref="M12:S13"/>
-    <mergeCell ref="T12:AB13"/>
-    <mergeCell ref="AC12:AM13"/>
-    <mergeCell ref="AR12:AT13"/>
-    <mergeCell ref="AU12:AW13"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="H10:L11"/>
-    <mergeCell ref="M10:S11"/>
-    <mergeCell ref="T10:AB11"/>
-    <mergeCell ref="BA8:BH8"/>
-    <mergeCell ref="AX8:AZ9"/>
-    <mergeCell ref="AU8:AW9"/>
-    <mergeCell ref="AR8:AT9"/>
-    <mergeCell ref="AN8:AQ9"/>
-    <mergeCell ref="BA9:BH9"/>
-    <mergeCell ref="AC8:AM9"/>
-    <mergeCell ref="AC10:AM11"/>
-    <mergeCell ref="AR10:AT11"/>
-    <mergeCell ref="AU10:AW11"/>
-    <mergeCell ref="AX10:AZ11"/>
-    <mergeCell ref="BA11:BH11"/>
-    <mergeCell ref="AN10:AQ11"/>
-    <mergeCell ref="AX12:AZ13"/>
-    <mergeCell ref="AN12:AQ13"/>
-    <mergeCell ref="BA13:BH13"/>
+    <mergeCell ref="AX18:AZ19"/>
+    <mergeCell ref="BA18:BH18"/>
+    <mergeCell ref="BA19:BH19"/>
+    <mergeCell ref="AX20:AZ21"/>
+    <mergeCell ref="BA20:BH20"/>
+    <mergeCell ref="BA21:BH21"/>
+    <mergeCell ref="AU16:AW17"/>
+    <mergeCell ref="AX14:AZ15"/>
+    <mergeCell ref="AX16:AZ17"/>
+    <mergeCell ref="BA16:BH16"/>
+    <mergeCell ref="BA17:BH17"/>
+    <mergeCell ref="BA14:BH14"/>
+    <mergeCell ref="BA15:BH15"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="H20:L21"/>
+    <mergeCell ref="M20:S21"/>
+    <mergeCell ref="T20:AB21"/>
+    <mergeCell ref="AC20:AM21"/>
+    <mergeCell ref="AN20:AQ21"/>
+    <mergeCell ref="AR20:AT21"/>
+    <mergeCell ref="AU20:AW21"/>
+    <mergeCell ref="C8:G21"/>
+    <mergeCell ref="AN18:AQ19"/>
+    <mergeCell ref="AR18:AT19"/>
+    <mergeCell ref="AU18:AW19"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="H14:L15"/>
+    <mergeCell ref="M14:S15"/>
+    <mergeCell ref="T14:AB15"/>
+    <mergeCell ref="AC14:AM15"/>
+    <mergeCell ref="H16:L17"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="M16:S17"/>
+    <mergeCell ref="T16:AB17"/>
+    <mergeCell ref="AC16:AM17"/>
+    <mergeCell ref="AN14:AQ15"/>
+    <mergeCell ref="AN16:AQ17"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR8 AR10 AR12 AR14 AR16 AR18 AR20">

</xml_diff>